<commit_message>
- Code refactoring - Converted JSON date strings into date time objects - Re-adjusted stock split price for Apple pricing
</commit_message>
<xml_diff>
--- a/stock_tracker.xlsx
+++ b/stock_tracker.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -53,9 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -159,7 +162,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Summary'!B1</f>
+              <f>'Summary'!A1</f>
             </strRef>
           </tx>
           <spPr>
@@ -184,7 +187,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Summary'!$B$2:$B$7</f>
+              <f>'Summary'!$A$2:$A$100</f>
             </numRef>
           </val>
         </ser>
@@ -193,7 +196,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Summary'!C1</f>
+              <f>'Summary'!B1</f>
             </strRef>
           </tx>
           <spPr>
@@ -214,7 +217,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Summary'!$C$2:$C$7</f>
+              <f>'Summary'!$B$2:$B$100</f>
             </numRef>
           </val>
         </ser>
@@ -223,7 +226,7 @@
           <order val="2"/>
           <tx>
             <strRef>
-              <f>'Summary'!D1</f>
+              <f>'Summary'!C1</f>
             </strRef>
           </tx>
           <spPr>
@@ -241,7 +244,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Summary'!$D$2:$D$7</f>
+              <f>'Summary'!$C$2:$C$100</f>
             </numRef>
           </val>
           <smooth val="1"/>
@@ -660,10 +663,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2020-12-28</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>44193</v>
       </c>
       <c r="B3" t="n">
         <v>137.34</v>
@@ -673,10 +674,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2020-12-24</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>44189</v>
       </c>
       <c r="B4" t="n">
         <v>133.46</v>
@@ -686,10 +685,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2020-12-23</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>44188</v>
       </c>
       <c r="B5" t="n">
         <v>132.43</v>
@@ -699,10 +696,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2020-12-22</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>44187</v>
       </c>
       <c r="B6" t="n">
         <v>134.405</v>
@@ -712,10 +707,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2020-12-21</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>44186</v>
       </c>
       <c r="B7" t="n">
         <v>128.31</v>
@@ -725,10 +718,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2020-12-18</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>44183</v>
       </c>
       <c r="B8" t="n">
         <v>129.1</v>
@@ -738,10 +729,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2020-12-17</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>44182</v>
       </c>
       <c r="B9" t="n">
         <v>129.58</v>
@@ -751,10 +740,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2020-12-16</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>44181</v>
       </c>
       <c r="B10" t="n">
         <v>128.37</v>
@@ -764,10 +751,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2020-12-15</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>44180</v>
       </c>
       <c r="B11" t="n">
         <v>127.9</v>
@@ -777,10 +762,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2020-12-14</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>44179</v>
       </c>
       <c r="B12" t="n">
         <v>123.35</v>
@@ -790,10 +773,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2020-12-11</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>44176</v>
       </c>
       <c r="B13" t="n">
         <v>122.76</v>
@@ -803,10 +784,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2020-12-10</t>
-        </is>
+      <c r="A14" s="2" t="n">
+        <v>44175</v>
       </c>
       <c r="B14" t="n">
         <v>123.87</v>
@@ -816,10 +795,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2020-12-09</t>
-        </is>
+      <c r="A15" s="2" t="n">
+        <v>44174</v>
       </c>
       <c r="B15" t="n">
         <v>125.95</v>
@@ -829,10 +806,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2020-12-08</t>
-        </is>
+      <c r="A16" s="2" t="n">
+        <v>44173</v>
       </c>
       <c r="B16" t="n">
         <v>124.98</v>
@@ -842,10 +817,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2020-12-07</t>
-        </is>
+      <c r="A17" s="2" t="n">
+        <v>44172</v>
       </c>
       <c r="B17" t="n">
         <v>124.57</v>
@@ -855,10 +828,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>2020-12-04</t>
-        </is>
+      <c r="A18" s="2" t="n">
+        <v>44169</v>
       </c>
       <c r="B18" t="n">
         <v>122.8608</v>
@@ -868,10 +839,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2020-12-03</t>
-        </is>
+      <c r="A19" s="2" t="n">
+        <v>44168</v>
       </c>
       <c r="B19" t="n">
         <v>123.78</v>
@@ -881,10 +850,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>2020-12-02</t>
-        </is>
+      <c r="A20" s="2" t="n">
+        <v>44167</v>
       </c>
       <c r="B20" t="n">
         <v>123.37</v>
@@ -894,10 +861,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>2020-12-01</t>
-        </is>
+      <c r="A21" s="2" t="n">
+        <v>44166</v>
       </c>
       <c r="B21" t="n">
         <v>123.4693</v>
@@ -907,10 +872,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>2020-11-30</t>
-        </is>
+      <c r="A22" s="2" t="n">
+        <v>44165</v>
       </c>
       <c r="B22" t="n">
         <v>120.97</v>
@@ -920,10 +883,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>2020-11-27</t>
-        </is>
+      <c r="A23" s="2" t="n">
+        <v>44162</v>
       </c>
       <c r="B23" t="n">
         <v>117.49</v>
@@ -933,10 +894,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2020-11-25</t>
-        </is>
+      <c r="A24" s="2" t="n">
+        <v>44160</v>
       </c>
       <c r="B24" t="n">
         <v>116.75</v>
@@ -946,10 +905,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2020-11-24</t>
-        </is>
+      <c r="A25" s="2" t="n">
+        <v>44159</v>
       </c>
       <c r="B25" t="n">
         <v>115.85</v>
@@ -959,10 +916,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2020-11-23</t>
-        </is>
+      <c r="A26" s="2" t="n">
+        <v>44158</v>
       </c>
       <c r="B26" t="n">
         <v>117.6202</v>
@@ -972,10 +927,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2020-11-20</t>
-        </is>
+      <c r="A27" s="2" t="n">
+        <v>44155</v>
       </c>
       <c r="B27" t="n">
         <v>118.77</v>
@@ -985,10 +938,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2020-11-19</t>
-        </is>
+      <c r="A28" s="2" t="n">
+        <v>44154</v>
       </c>
       <c r="B28" t="n">
         <v>119.06</v>
@@ -998,10 +949,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2020-11-18</t>
-        </is>
+      <c r="A29" s="2" t="n">
+        <v>44153</v>
       </c>
       <c r="B29" t="n">
         <v>119.82</v>
@@ -1011,10 +960,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2020-11-17</t>
-        </is>
+      <c r="A30" s="2" t="n">
+        <v>44152</v>
       </c>
       <c r="B30" t="n">
         <v>120.6741</v>
@@ -1024,10 +971,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2020-11-16</t>
-        </is>
+      <c r="A31" s="2" t="n">
+        <v>44151</v>
       </c>
       <c r="B31" t="n">
         <v>120.99</v>
@@ -1037,10 +982,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2020-11-13</t>
-        </is>
+      <c r="A32" s="2" t="n">
+        <v>44148</v>
       </c>
       <c r="B32" t="n">
         <v>119.6717</v>
@@ -1050,10 +993,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2020-11-12</t>
-        </is>
+      <c r="A33" s="2" t="n">
+        <v>44147</v>
       </c>
       <c r="B33" t="n">
         <v>120.53</v>
@@ -1063,10 +1004,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2020-11-11</t>
-        </is>
+      <c r="A34" s="2" t="n">
+        <v>44146</v>
       </c>
       <c r="B34" t="n">
         <v>119.63</v>
@@ -1076,10 +1015,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2020-11-10</t>
-        </is>
+      <c r="A35" s="2" t="n">
+        <v>44145</v>
       </c>
       <c r="B35" t="n">
         <v>117.59</v>
@@ -1089,10 +1026,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2020-11-09</t>
-        </is>
+      <c r="A36" s="2" t="n">
+        <v>44144</v>
       </c>
       <c r="B36" t="n">
         <v>121.99</v>
@@ -1102,10 +1037,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2020-11-06</t>
-        </is>
+      <c r="A37" s="2" t="n">
+        <v>44141</v>
       </c>
       <c r="B37" t="n">
         <v>119.2</v>
@@ -1115,10 +1048,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2020-11-05</t>
-        </is>
+      <c r="A38" s="2" t="n">
+        <v>44140</v>
       </c>
       <c r="B38" t="n">
         <v>119.62</v>
@@ -1128,10 +1059,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>2020-11-04</t>
-        </is>
+      <c r="A39" s="2" t="n">
+        <v>44139</v>
       </c>
       <c r="B39" t="n">
         <v>115.59</v>
@@ -1141,10 +1070,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>2020-11-03</t>
-        </is>
+      <c r="A40" s="2" t="n">
+        <v>44138</v>
       </c>
       <c r="B40" t="n">
         <v>111.49</v>
@@ -1154,10 +1081,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>2020-11-02</t>
-        </is>
+      <c r="A41" s="2" t="n">
+        <v>44137</v>
       </c>
       <c r="B41" t="n">
         <v>110.68</v>
@@ -1167,10 +1092,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2020-10-30</t>
-        </is>
+      <c r="A42" s="2" t="n">
+        <v>44134</v>
       </c>
       <c r="B42" t="n">
         <v>111.99</v>
@@ -1180,10 +1103,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2020-10-29</t>
-        </is>
+      <c r="A43" s="2" t="n">
+        <v>44133</v>
       </c>
       <c r="B43" t="n">
         <v>116.93</v>
@@ -1193,10 +1114,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2020-10-28</t>
-        </is>
+      <c r="A44" s="2" t="n">
+        <v>44132</v>
       </c>
       <c r="B44" t="n">
         <v>115.43</v>
@@ -1206,10 +1125,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2020-10-27</t>
-        </is>
+      <c r="A45" s="2" t="n">
+        <v>44131</v>
       </c>
       <c r="B45" t="n">
         <v>117.28</v>
@@ -1219,10 +1136,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>2020-10-26</t>
-        </is>
+      <c r="A46" s="2" t="n">
+        <v>44130</v>
       </c>
       <c r="B46" t="n">
         <v>116.55</v>
@@ -1232,10 +1147,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>2020-10-23</t>
-        </is>
+      <c r="A47" s="2" t="n">
+        <v>44127</v>
       </c>
       <c r="B47" t="n">
         <v>116.55</v>
@@ -1245,10 +1158,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>2020-10-22</t>
-        </is>
+      <c r="A48" s="2" t="n">
+        <v>44126</v>
       </c>
       <c r="B48" t="n">
         <v>118.04</v>
@@ -1258,10 +1169,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>2020-10-21</t>
-        </is>
+      <c r="A49" s="2" t="n">
+        <v>44125</v>
       </c>
       <c r="B49" t="n">
         <v>118.705</v>
@@ -1271,10 +1180,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>2020-10-20</t>
-        </is>
+      <c r="A50" s="2" t="n">
+        <v>44124</v>
       </c>
       <c r="B50" t="n">
         <v>118.98</v>
@@ -1284,10 +1191,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>2020-10-19</t>
-        </is>
+      <c r="A51" s="2" t="n">
+        <v>44123</v>
       </c>
       <c r="B51" t="n">
         <v>120.419</v>
@@ -1297,10 +1202,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>2020-10-16</t>
-        </is>
+      <c r="A52" s="2" t="n">
+        <v>44120</v>
       </c>
       <c r="B52" t="n">
         <v>121.548</v>
@@ -1310,10 +1213,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>2020-10-15</t>
-        </is>
+      <c r="A53" s="2" t="n">
+        <v>44119</v>
       </c>
       <c r="B53" t="n">
         <v>121.2</v>
@@ -1323,10 +1224,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>2020-10-14</t>
-        </is>
+      <c r="A54" s="2" t="n">
+        <v>44118</v>
       </c>
       <c r="B54" t="n">
         <v>123.03</v>
@@ -1336,10 +1235,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>2020-10-13</t>
-        </is>
+      <c r="A55" s="2" t="n">
+        <v>44117</v>
       </c>
       <c r="B55" t="n">
         <v>125.39</v>
@@ -1349,10 +1246,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>2020-10-12</t>
-        </is>
+      <c r="A56" s="2" t="n">
+        <v>44116</v>
       </c>
       <c r="B56" t="n">
         <v>125.18</v>
@@ -1362,10 +1257,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>2020-10-09</t>
-        </is>
+      <c r="A57" s="2" t="n">
+        <v>44113</v>
       </c>
       <c r="B57" t="n">
         <v>117</v>
@@ -1375,10 +1268,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2020-10-08</t>
-        </is>
+      <c r="A58" s="2" t="n">
+        <v>44112</v>
       </c>
       <c r="B58" t="n">
         <v>116.4</v>
@@ -1388,10 +1279,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>2020-10-07</t>
-        </is>
+      <c r="A59" s="2" t="n">
+        <v>44111</v>
       </c>
       <c r="B59" t="n">
         <v>115.55</v>
@@ -1401,10 +1290,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>2020-10-06</t>
-        </is>
+      <c r="A60" s="2" t="n">
+        <v>44110</v>
       </c>
       <c r="B60" t="n">
         <v>116.12</v>
@@ -1414,10 +1301,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>2020-10-05</t>
-        </is>
+      <c r="A61" s="2" t="n">
+        <v>44109</v>
       </c>
       <c r="B61" t="n">
         <v>116.65</v>
@@ -1427,10 +1312,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>2020-10-02</t>
-        </is>
+      <c r="A62" s="2" t="n">
+        <v>44106</v>
       </c>
       <c r="B62" t="n">
         <v>115.37</v>
@@ -1440,10 +1323,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>2020-10-01</t>
-        </is>
+      <c r="A63" s="2" t="n">
+        <v>44105</v>
       </c>
       <c r="B63" t="n">
         <v>117.72</v>
@@ -1453,10 +1334,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>2020-09-30</t>
-        </is>
+      <c r="A64" s="2" t="n">
+        <v>44104</v>
       </c>
       <c r="B64" t="n">
         <v>117.26</v>
@@ -1466,10 +1345,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>2020-09-29</t>
-        </is>
+      <c r="A65" s="2" t="n">
+        <v>44103</v>
       </c>
       <c r="B65" t="n">
         <v>115.31</v>
@@ -1479,10 +1356,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>2020-09-28</t>
-        </is>
+      <c r="A66" s="2" t="n">
+        <v>44102</v>
       </c>
       <c r="B66" t="n">
         <v>115.32</v>
@@ -1492,10 +1367,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>2020-09-25</t>
-        </is>
+      <c r="A67" s="2" t="n">
+        <v>44099</v>
       </c>
       <c r="B67" t="n">
         <v>112.44</v>
@@ -1505,10 +1378,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>2020-09-24</t>
-        </is>
+      <c r="A68" s="2" t="n">
+        <v>44098</v>
       </c>
       <c r="B68" t="n">
         <v>110.25</v>
@@ -1518,10 +1389,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>2020-09-23</t>
-        </is>
+      <c r="A69" s="2" t="n">
+        <v>44097</v>
       </c>
       <c r="B69" t="n">
         <v>112.11</v>
@@ -1531,10 +1400,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>2020-09-22</t>
-        </is>
+      <c r="A70" s="2" t="n">
+        <v>44096</v>
       </c>
       <c r="B70" t="n">
         <v>112.86</v>
@@ -1544,10 +1411,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>2020-09-21</t>
-        </is>
+      <c r="A71" s="2" t="n">
+        <v>44095</v>
       </c>
       <c r="B71" t="n">
         <v>110.19</v>
@@ -1557,10 +1422,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>2020-09-18</t>
-        </is>
+      <c r="A72" s="2" t="n">
+        <v>44092</v>
       </c>
       <c r="B72" t="n">
         <v>110.88</v>
@@ -1570,10 +1433,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>2020-09-17</t>
-        </is>
+      <c r="A73" s="2" t="n">
+        <v>44091</v>
       </c>
       <c r="B73" t="n">
         <v>112.2</v>
@@ -1583,10 +1444,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>2020-09-16</t>
-        </is>
+      <c r="A74" s="2" t="n">
+        <v>44090</v>
       </c>
       <c r="B74" t="n">
         <v>116</v>
@@ -1596,10 +1455,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>2020-09-15</t>
-        </is>
+      <c r="A75" s="2" t="n">
+        <v>44089</v>
       </c>
       <c r="B75" t="n">
         <v>118.829</v>
@@ -1609,10 +1466,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>2020-09-14</t>
-        </is>
+      <c r="A76" s="2" t="n">
+        <v>44088</v>
       </c>
       <c r="B76" t="n">
         <v>115.93</v>
@@ -1622,10 +1477,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>2020-09-11</t>
-        </is>
+      <c r="A77" s="2" t="n">
+        <v>44085</v>
       </c>
       <c r="B77" t="n">
         <v>115.23</v>
@@ -1635,10 +1488,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>2020-09-10</t>
-        </is>
+      <c r="A78" s="2" t="n">
+        <v>44084</v>
       </c>
       <c r="B78" t="n">
         <v>120.5</v>
@@ -1648,10 +1499,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>2020-09-09</t>
-        </is>
+      <c r="A79" s="2" t="n">
+        <v>44083</v>
       </c>
       <c r="B79" t="n">
         <v>119.14</v>
@@ -1661,10 +1510,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>2020-09-08</t>
-        </is>
+      <c r="A80" s="2" t="n">
+        <v>44082</v>
       </c>
       <c r="B80" t="n">
         <v>118.99</v>
@@ -1674,10 +1521,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>2020-09-04</t>
-        </is>
+      <c r="A81" s="2" t="n">
+        <v>44078</v>
       </c>
       <c r="B81" t="n">
         <v>123.7</v>
@@ -1687,10 +1532,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>2020-09-03</t>
-        </is>
+      <c r="A82" s="2" t="n">
+        <v>44077</v>
       </c>
       <c r="B82" t="n">
         <v>128.84</v>
@@ -1700,10 +1543,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>2020-09-02</t>
-        </is>
+      <c r="A83" s="2" t="n">
+        <v>44076</v>
       </c>
       <c r="B83" t="n">
         <v>137.98</v>
@@ -1713,10 +1554,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>2020-09-01</t>
-        </is>
+      <c r="A84" s="2" t="n">
+        <v>44075</v>
       </c>
       <c r="B84" t="n">
         <v>134.8</v>
@@ -1726,10 +1565,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>2020-08-31</t>
-        </is>
+      <c r="A85" s="2" t="n">
+        <v>44074</v>
       </c>
       <c r="B85" t="n">
         <v>131</v>
@@ -1739,10 +1576,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>2020-08-28</t>
-        </is>
+      <c r="A86" s="2" t="n">
+        <v>44071</v>
       </c>
       <c r="B86" t="n">
         <v>505.77</v>
@@ -1752,211 +1587,179 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>2020-08-27</t>
-        </is>
+      <c r="A87" s="2" t="n">
+        <v>44070</v>
       </c>
       <c r="B87" t="n">
-        <v>509.94</v>
+        <v>127.485</v>
       </c>
       <c r="C87" t="n">
-        <v>495.33</v>
+        <v>123.8325</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>2020-08-26</t>
-        </is>
+      <c r="A88" s="2" t="n">
+        <v>44069</v>
       </c>
       <c r="B88" t="n">
-        <v>507.97</v>
+        <v>126.9925</v>
       </c>
       <c r="C88" t="n">
-        <v>500.33</v>
+        <v>125.0825</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>2020-08-25</t>
-        </is>
+      <c r="A89" s="2" t="n">
+        <v>44068</v>
       </c>
       <c r="B89" t="n">
-        <v>500.7172</v>
+        <v>125.1793</v>
       </c>
       <c r="C89" t="n">
-        <v>492.21</v>
+        <v>123.0525</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>2020-08-24</t>
-        </is>
+      <c r="A90" s="2" t="n">
+        <v>44067</v>
       </c>
       <c r="B90" t="n">
-        <v>515.14</v>
+        <v>128.785</v>
       </c>
       <c r="C90" t="n">
-        <v>495.745</v>
+        <v>123.93625</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>2020-08-21</t>
-        </is>
+      <c r="A91" s="2" t="n">
+        <v>44064</v>
       </c>
       <c r="B91" t="n">
-        <v>499.472</v>
+        <v>124.868</v>
       </c>
       <c r="C91" t="n">
-        <v>477</v>
+        <v>119.25</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>2020-08-20</t>
-        </is>
+      <c r="A92" s="2" t="n">
+        <v>44063</v>
       </c>
       <c r="B92" t="n">
-        <v>473.568</v>
+        <v>118.392</v>
       </c>
       <c r="C92" t="n">
-        <v>462.9335</v>
+        <v>115.733375</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>2020-08-19</t>
-        </is>
+      <c r="A93" s="2" t="n">
+        <v>44062</v>
       </c>
       <c r="B93" t="n">
-        <v>468.65</v>
+        <v>117.1625</v>
       </c>
       <c r="C93" t="n">
-        <v>462.44</v>
+        <v>115.61</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>2020-08-18</t>
-        </is>
+      <c r="A94" s="2" t="n">
+        <v>44061</v>
       </c>
       <c r="B94" t="n">
-        <v>464</v>
+        <v>116</v>
       </c>
       <c r="C94" t="n">
-        <v>456.03</v>
+        <v>114.0075</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>2020-08-17</t>
-        </is>
+      <c r="A95" s="2" t="n">
+        <v>44060</v>
       </c>
       <c r="B95" t="n">
-        <v>464.35</v>
+        <v>116.0875</v>
       </c>
       <c r="C95" t="n">
-        <v>455.8501</v>
+        <v>113.962525</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>2020-08-14</t>
-        </is>
+      <c r="A96" s="2" t="n">
+        <v>44057</v>
       </c>
       <c r="B96" t="n">
-        <v>460</v>
+        <v>115</v>
       </c>
       <c r="C96" t="n">
-        <v>452.18</v>
+        <v>113.045</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>2020-08-13</t>
-        </is>
+      <c r="A97" s="2" t="n">
+        <v>44056</v>
       </c>
       <c r="B97" t="n">
-        <v>464.17</v>
+        <v>116.0425</v>
       </c>
       <c r="C97" t="n">
-        <v>455.71</v>
+        <v>113.9275</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>2020-08-12</t>
-        </is>
+      <c r="A98" s="2" t="n">
+        <v>44055</v>
       </c>
       <c r="B98" t="n">
-        <v>453.1</v>
+        <v>113.275</v>
       </c>
       <c r="C98" t="n">
-        <v>441.19</v>
+        <v>110.2975</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>2020-08-11</t>
-        </is>
+      <c r="A99" s="2" t="n">
+        <v>44054</v>
       </c>
       <c r="B99" t="n">
-        <v>449.93</v>
+        <v>112.4825</v>
       </c>
       <c r="C99" t="n">
-        <v>436.4267</v>
+        <v>109.106675</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>2020-08-10</t>
-        </is>
+      <c r="A100" s="2" t="n">
+        <v>44053</v>
       </c>
       <c r="B100" t="n">
-        <v>455.1</v>
+        <v>113.775</v>
       </c>
       <c r="C100" t="n">
-        <v>440</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>2020-08-07</t>
-        </is>
+      <c r="A101" s="2" t="n">
+        <v>44050</v>
       </c>
       <c r="B101" t="n">
-        <v>454.7</v>
+        <v>113.675</v>
       </c>
       <c r="C101" t="n">
-        <v>441.17</v>
+        <v>110.2925</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>2020-08-06</t>
-        </is>
+      <c r="A102" s="2" t="n">
+        <v>44049</v>
       </c>
       <c r="B102" t="n">
-        <v>457.65</v>
+        <v>114.4125</v>
       </c>
       <c r="C102" t="n">
-        <v>439.19</v>
+        <v>109.7975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Chart changes and more code refactoring. - Self score, 3/10: future TODOs would improve.
</commit_message>
<xml_diff>
--- a/stock_tracker.xlsx
+++ b/stock_tracker.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Apple Tab" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Apple" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tesla" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -148,7 +148,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Test Chart</a:t>
+              <a:t>Apple Highs vs Lows</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -162,7 +162,34 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Summary'!A1</f>
+              <f>'Apple'!B2</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'Apple'!$B$3:$B$105</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Apple'!C2</f>
             </strRef>
           </tx>
           <spPr>
@@ -187,16 +214,16 @@
           </marker>
           <val>
             <numRef>
-              <f>'Summary'!$A$2:$A$100</f>
+              <f>'Apple'!$C$3:$C$105</f>
             </numRef>
           </val>
         </ser>
         <ser>
-          <idx val="1"/>
-          <order val="1"/>
+          <idx val="2"/>
+          <order val="2"/>
           <tx>
             <strRef>
-              <f>'Summary'!B1</f>
+              <f>'Apple'!D2</f>
             </strRef>
           </tx>
           <spPr>
@@ -217,34 +244,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Summary'!$B$2:$B$100</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'Summary'!C1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'Summary'!$C$2:$C$100</f>
+              <f>'Apple'!$D$3:$D$105</f>
             </numRef>
           </val>
           <smooth val="1"/>
@@ -267,7 +267,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Test Number</a:t>
+                  <a:t>Date</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -282,6 +282,8 @@
         <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
+          <max val="140"/>
+          <min val="100"/>
         </scaling>
         <axPos val="l"/>
         <majorGridlines/>
@@ -294,7 +296,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:t>Size</a:t>
+                  <a:t>Price</a:t>
                 </a:r>
               </a:p>
             </rich>
@@ -320,10 +322,10 @@
     <from>
       <col>4</col>
       <colOff>0</colOff>
-      <row>9</row>
+      <row>4</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="2700000"/>
+    <ext cx="10800000" cy="5400000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -641,7 +643,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Summary Page</t>
+          <t>Apple Data</t>
         </is>
       </c>
     </row>
@@ -1580,10 +1582,10 @@
         <v>44071</v>
       </c>
       <c r="B86" t="n">
-        <v>505.77</v>
+        <v>126.4425</v>
       </c>
       <c r="C86" t="n">
-        <v>498.31</v>
+        <v>124.5775</v>
       </c>
     </row>
     <row r="87">
@@ -1785,7 +1787,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Apple raw data</t>
+          <t>Tesla Data</t>
         </is>
       </c>
     </row>

</xml_diff>